<commit_message>
Updates exercises, deletes excess files
</commit_message>
<xml_diff>
--- a/04_Exercises/Training_QC_dicoms/QC_Test_Key.xlsx
+++ b/04_Exercises/Training_QC_dicoms/QC_Test_Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/vdrive/helpern_playarea/mcgill_c/QC_Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kayti/Library/Containers/com.microsoft.Excel/Data/Desktop/Projects/Analysis-Docs/04_Exercises/Training_QC_dicoms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29B0CA1-446E-1244-B578-E759FD270D15}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169F6E93-CBF0-FA4D-A03C-97BE8AB4F631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76820" yWindow="480" windowWidth="25600" windowHeight="28340" activeTab="1" xr2:uid="{6022A857-F787-F84B-9BAF-9623F16107C5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17560" windowHeight="16600" activeTab="1" xr2:uid="{6022A857-F787-F84B-9BAF-9623F16107C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Good 201, 202, 201_FU, 203, 201</t>
   </si>
@@ -46,9 +46,6 @@
     <t>MIND ID</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -61,28 +58,13 @@
     <t>C</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>J</t>
-  </si>
-  <si>
-    <t>201_FU</t>
   </si>
   <si>
     <t>1- mild</t>
@@ -95,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -467,14 +449,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -486,13 +468,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3F4996-DA82-D245-9186-59398004F3B8}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -500,7 +482,7 @@
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -514,155 +496,85 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>201</v>
+        <v>263</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>263</v>
+        <v>206</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>220</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>208</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>220</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>216</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>245</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>218</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>